<commit_message>
lecture 7 and section 2
</commit_message>
<xml_diff>
--- a/teaching/ClassRoster.xlsx
+++ b/teaching/ClassRoster.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/classes/teaching/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Last</t>
   </si>
@@ -33,9 +41,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Morley</t>
   </si>
   <si>
@@ -139,6 +144,15 @@
   </si>
   <si>
     <t>Steinberg</t>
+  </si>
+  <si>
+    <t>Section 1</t>
+  </si>
+  <si>
+    <t>Section 2</t>
+  </si>
+  <si>
+    <t>Abs</t>
   </si>
 </sst>
 </file>
@@ -182,6 +196,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -507,15 +526,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,239 +548,333 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2">
         <v>11170501</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
       <c r="D3">
         <v>60977623</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>41170549</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>31238749</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6">
         <v>60983771</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>51170806</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <v>90977989</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9">
         <v>41292679</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>50977277</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>71292320</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <v>20983248</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13">
         <v>11312357</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <v>20944080</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15">
         <v>21292079</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
       </c>
       <c r="D16">
         <v>21368318</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17">
         <v>21291951</v>
       </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lecture 9 and attendance
</commit_message>
<xml_diff>
--- a/teaching/ClassRoster.xlsx
+++ b/teaching/ClassRoster.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>Last</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Abs</t>
+  </si>
+  <si>
+    <t>MCZ Tours</t>
   </si>
 </sst>
 </file>
@@ -526,15 +529,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,8 +556,11 @@
       <c r="F1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -573,8 +579,11 @@
       <c r="F2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -593,8 +602,11 @@
       <c r="F3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -613,8 +625,11 @@
       <c r="F4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -633,8 +648,11 @@
       <c r="F5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -653,8 +671,11 @@
       <c r="F6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -673,8 +694,11 @@
       <c r="F7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -693,8 +717,11 @@
       <c r="F8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -713,8 +740,11 @@
       <c r="F9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -733,8 +763,11 @@
       <c r="F10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -753,8 +786,11 @@
       <c r="F11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -773,8 +809,11 @@
       <c r="F12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -793,8 +832,11 @@
       <c r="F13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -813,8 +855,11 @@
       <c r="F14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -833,8 +878,11 @@
       <c r="F15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -853,8 +901,11 @@
       <c r="F16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -871,6 +922,9 @@
         <v>2</v>
       </c>
       <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lecture 14 and 15
</commit_message>
<xml_diff>
--- a/teaching/ClassRoster.xlsx
+++ b/teaching/ClassRoster.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/classes/teaching/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="600" yWindow="0" windowWidth="23280" windowHeight="10540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>Last</t>
   </si>
@@ -165,6 +160,15 @@
   </si>
   <si>
     <t>Section 5</t>
+  </si>
+  <si>
+    <t>Section 6</t>
+  </si>
+  <si>
+    <t>P-Set 1</t>
+  </si>
+  <si>
+    <t>Told Score</t>
   </si>
 </sst>
 </file>
@@ -538,15 +542,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,8 +581,17 @@
       <c r="J1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -609,8 +622,17 @@
       <c r="J2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>29</v>
+      </c>
+      <c r="M2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -641,8 +663,17 @@
       <c r="J3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>29</v>
+      </c>
+      <c r="M3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -673,8 +704,17 @@
       <c r="J4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>30</v>
+      </c>
+      <c r="M4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -705,8 +745,17 @@
       <c r="J5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>29</v>
+      </c>
+      <c r="M5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -737,8 +786,17 @@
       <c r="J6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>28</v>
+      </c>
+      <c r="M6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -769,8 +827,17 @@
       <c r="J7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -801,8 +868,17 @@
       <c r="J8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>27</v>
+      </c>
+      <c r="M8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -833,8 +909,17 @@
       <c r="J9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>30</v>
+      </c>
+      <c r="M9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -865,8 +950,17 @@
       <c r="J10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>29</v>
+      </c>
+      <c r="M10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -897,8 +991,14 @@
       <c r="J11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -929,8 +1029,17 @@
       <c r="J12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <v>30</v>
+      </c>
+      <c r="M12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -961,8 +1070,17 @@
       <c r="J13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>30</v>
+      </c>
+      <c r="M13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -993,8 +1111,14 @@
       <c r="J14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1025,8 +1149,14 @@
       <c r="J15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1057,8 +1187,17 @@
       <c r="J16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>30</v>
+      </c>
+      <c r="M16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1088,6 +1227,15 @@
       </c>
       <c r="J17">
         <v>2</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>29</v>
+      </c>
+      <c r="M17">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1095,5 +1243,10 @@
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated roster and lectures
</commit_message>
<xml_diff>
--- a/teaching/ClassRoster.xlsx
+++ b/teaching/ClassRoster.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/classes/teaching/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="0" windowWidth="23280" windowHeight="10540" tabRatio="500"/>
+    <workbookView xWindow="2320" yWindow="460" windowWidth="23280" windowHeight="10540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>Last</t>
   </si>
@@ -166,6 +171,12 @@
   </si>
   <si>
     <t>P-Set 1</t>
+  </si>
+  <si>
+    <t>Section 7</t>
+  </si>
+  <si>
+    <t>MidTerm2</t>
   </si>
 </sst>
 </file>
@@ -539,18 +550,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="11" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -587,8 +598,14 @@
       <c r="L1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -625,8 +642,14 @@
       <c r="L2">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>53.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -663,8 +686,14 @@
       <c r="L3">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -701,8 +730,14 @@
       <c r="L4">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -739,8 +774,14 @@
       <c r="L5">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -777,8 +818,14 @@
       <c r="L6">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -815,8 +862,14 @@
       <c r="L7">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -853,8 +906,14 @@
       <c r="L8">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -891,8 +950,14 @@
       <c r="L9">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -929,8 +994,14 @@
       <c r="L10">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -967,8 +1038,14 @@
       <c r="L11">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1005,8 +1082,14 @@
       <c r="L12">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1043,8 +1126,14 @@
       <c r="L13">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1081,8 +1170,14 @@
       <c r="L14">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1119,8 +1214,14 @@
       <c r="L15">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1157,8 +1258,14 @@
       <c r="L16">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1194,6 +1301,12 @@
       </c>
       <c r="L17">
         <v>29</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1201,10 +1314,5 @@
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>